<commit_message>
Offers: Content - Replaced Dark by Devil and Alien by Chinese dragons in the playtest offer packs.
Former-commit-id: 2d95df22e5bf563ffd2d703d184191219003f214
</commit_message>
<xml_diff>
--- a/Docs/Content/HungryDragonContent_Offers_SHOP_PLAYTEST.xlsx
+++ b/Docs/Content/HungryDragonContent_Offers_SHOP_PLAYTEST.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/aortin/Documents/UBI/FD/Client_iOS/Docs/Content/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{514C0998-AC50-F343-956C-C6EFC229DE78}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DBD05BB2-6178-044E-A14D-8AC14CB917E5}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="460" windowWidth="38400" windowHeight="23540" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3702" uniqueCount="407">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3702" uniqueCount="408">
   <si>
     <t>[sku]</t>
   </si>
@@ -1221,18 +1221,12 @@
     <t>0:999</t>
   </si>
   <si>
-    <t>dragon_dark_1</t>
-  </si>
-  <si>
     <t>TID_OFFER_PLAYTEST_2</t>
   </si>
   <si>
     <t>TID_OFFER_PLAYTEST_3</t>
   </si>
   <si>
-    <t>dragon_alien_3</t>
-  </si>
-  <si>
     <t>TID_OFFER_PLAYTEST_4</t>
   </si>
   <si>
@@ -1249,6 +1243,15 @@
   </si>
   <si>
     <t>TID_OFFER_PLAYTEST_9</t>
+  </si>
+  <si>
+    <t>dragon_devil</t>
+  </si>
+  <si>
+    <t>dragon_devil_1</t>
+  </si>
+  <si>
+    <t>dragon_devil_3</t>
   </si>
 </sst>
 </file>
@@ -2656,6 +2659,324 @@
     <xf numFmtId="0" fontId="2" fillId="22" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="14" fillId="12" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="14" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="19" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="15" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="14" fillId="7" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="7" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="7" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="7" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="5" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="5" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="24" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="5" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="12" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="14" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="19" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="15" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="23" fillId="7" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="14" fillId="22" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="24" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="7" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="7" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="11" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="9" borderId="5" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="9" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="9" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="6" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="6" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="6" borderId="5" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="23" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="13" fillId="6" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="24" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="22" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="5" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="24" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="5" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="22" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="5" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="24" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="5" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="22" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="5" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="5" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="24" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="22" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="5" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="22" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="22" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="5" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="5" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="22" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="5" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="22" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="5" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="24" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="24" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="22" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="24" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="22" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="12" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="24" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="22" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="14" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="24" borderId="12" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="19" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="15" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="24" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="24" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="22" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="7" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="22" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="7" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="14" fillId="24" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="23" fillId="7" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="14" fillId="22" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="23" fillId="7" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="24" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="22" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="7" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="24" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="22" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="24" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="22" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="7" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="24" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="22" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="24" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="22" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="7" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="24" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="22" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="24" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="24" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="22" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="11" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="22" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="9" borderId="13" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="9" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="25" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="6" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="25" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="23" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="6" borderId="13" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -2669,324 +2990,6 @@
       <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="12" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="14" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="19" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="15" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="14" fillId="7" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="7" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="7" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="7" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="5" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="5" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="24" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="5" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="12" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="14" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="19" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="15" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="23" fillId="7" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="14" fillId="22" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="24" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="7" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="7" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="11" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="9" borderId="5" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="9" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="9" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="6" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="6" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="6" borderId="5" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="23" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="13" fillId="6" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="24" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="22" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="5" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="24" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="5" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="22" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="5" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="24" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="5" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="5" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="22" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="5" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="5" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="24" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="5" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="22" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="5" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="5" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="22" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="5" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="22" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="5" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="5" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="22" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="5" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="22" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="5" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="24" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="24" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="22" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="24" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="22" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="12" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="24" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="22" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="14" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="24" borderId="12" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="19" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="15" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="24" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="24" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="22" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="7" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="22" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="7" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="14" fillId="24" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="23" fillId="7" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="14" fillId="22" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="23" fillId="7" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="24" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="22" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="7" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="24" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="22" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="24" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="22" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="7" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="24" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="22" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="24" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="22" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="7" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="24" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="22" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="24" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="24" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="22" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="11" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="22" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="9" borderId="13" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="9" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="25" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="6" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="25" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="23" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="6" borderId="13" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -6471,8 +6474,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="B1:BE94"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="L6" sqref="L6"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="O12" sqref="O12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16"/>
@@ -6536,41 +6539,41 @@
       <c r="V1" s="142" t="s">
         <v>292</v>
       </c>
-      <c r="AA1" s="256" t="s">
+      <c r="AA1" s="362" t="s">
         <v>77</v>
       </c>
-      <c r="AB1" s="256"/>
+      <c r="AB1" s="362"/>
       <c r="AC1" s="18"/>
-      <c r="AD1" s="257" t="s">
+      <c r="AD1" s="363" t="s">
         <v>76</v>
       </c>
-      <c r="AE1" s="257"/>
-      <c r="AF1" s="257"/>
-      <c r="AG1" s="257"/>
-      <c r="AH1" s="257"/>
-      <c r="AI1" s="257"/>
-      <c r="AJ1" s="257"/>
-      <c r="AK1" s="257"/>
-      <c r="AL1" s="257"/>
-      <c r="AM1" s="257"/>
-      <c r="AN1" s="257"/>
-      <c r="AO1" s="257"/>
-      <c r="AP1" s="257"/>
-      <c r="AQ1" s="257"/>
-      <c r="AR1" s="257"/>
-      <c r="AS1" s="257"/>
-      <c r="AT1" s="257"/>
-      <c r="AU1" s="257"/>
-      <c r="AV1" s="257"/>
-      <c r="AW1" s="257"/>
-      <c r="AX1" s="257"/>
-      <c r="AY1" s="257"/>
-      <c r="BA1" s="259" t="s">
+      <c r="AE1" s="363"/>
+      <c r="AF1" s="363"/>
+      <c r="AG1" s="363"/>
+      <c r="AH1" s="363"/>
+      <c r="AI1" s="363"/>
+      <c r="AJ1" s="363"/>
+      <c r="AK1" s="363"/>
+      <c r="AL1" s="363"/>
+      <c r="AM1" s="363"/>
+      <c r="AN1" s="363"/>
+      <c r="AO1" s="363"/>
+      <c r="AP1" s="363"/>
+      <c r="AQ1" s="363"/>
+      <c r="AR1" s="363"/>
+      <c r="AS1" s="363"/>
+      <c r="AT1" s="363"/>
+      <c r="AU1" s="363"/>
+      <c r="AV1" s="363"/>
+      <c r="AW1" s="363"/>
+      <c r="AX1" s="363"/>
+      <c r="AY1" s="363"/>
+      <c r="BA1" s="365" t="s">
         <v>382</v>
       </c>
-      <c r="BB1" s="260"/>
-      <c r="BC1" s="260"/>
-      <c r="BD1" s="260"/>
+      <c r="BB1" s="366"/>
+      <c r="BC1" s="366"/>
+      <c r="BD1" s="366"/>
       <c r="BE1" s="185"/>
     </row>
     <row r="2" spans="2:57" ht="149" customHeight="1">
@@ -7269,7 +7272,7 @@
       <c r="F6" s="225" t="s">
         <v>391</v>
       </c>
-      <c r="G6" s="322" t="b">
+      <c r="G6" s="317" t="b">
         <v>1</v>
       </c>
       <c r="H6" s="212">
@@ -7309,7 +7312,7 @@
         <v>88</v>
       </c>
       <c r="X6" s="217" t="s">
-        <v>402</v>
+        <v>400</v>
       </c>
       <c r="Y6" s="233" t="b">
         <v>1</v>
@@ -7330,8 +7333,8 @@
         <v>126</v>
       </c>
       <c r="AE6" s="219">
-        <f ca="1">RANDBETWEEN(5,1440)</f>
-        <v>775</v>
+        <f t="shared" ref="AE6:AE14" ca="1" si="0">RANDBETWEEN(5,1440)</f>
+        <v>1262</v>
       </c>
       <c r="AF6" s="220" t="s">
         <v>347</v>
@@ -7428,7 +7431,7 @@
       <c r="F7" s="225" t="s">
         <v>391</v>
       </c>
-      <c r="G7" s="322" t="b">
+      <c r="G7" s="317" t="b">
         <v>1</v>
       </c>
       <c r="H7" s="212">
@@ -7480,7 +7483,7 @@
         <v>91</v>
       </c>
       <c r="X7" s="217" t="s">
-        <v>403</v>
+        <v>401</v>
       </c>
       <c r="Y7" s="233" t="b">
         <v>1</v>
@@ -7501,8 +7504,8 @@
         <v>126</v>
       </c>
       <c r="AE7" s="219">
-        <f ca="1">RANDBETWEEN(5,1440)</f>
-        <v>754</v>
+        <f t="shared" ca="1" si="0"/>
+        <v>788</v>
       </c>
       <c r="AF7" s="220" t="s">
         <v>347</v>
@@ -7599,7 +7602,7 @@
       <c r="F8" s="225" t="s">
         <v>391</v>
       </c>
-      <c r="G8" s="322" t="b">
+      <c r="G8" s="317" t="b">
         <v>1</v>
       </c>
       <c r="H8" s="212">
@@ -7637,7 +7640,7 @@
         <v>257</v>
       </c>
       <c r="X8" s="217" t="s">
-        <v>404</v>
+        <v>402</v>
       </c>
       <c r="Y8" s="219" t="b">
         <v>1</v>
@@ -7658,8 +7661,8 @@
         <v>126</v>
       </c>
       <c r="AE8" s="219">
-        <f ca="1">RANDBETWEEN(5,1440)</f>
-        <v>1236</v>
+        <f t="shared" ca="1" si="0"/>
+        <v>468</v>
       </c>
       <c r="AF8" s="220" t="s">
         <v>347</v>
@@ -7756,7 +7759,7 @@
       <c r="F9" s="225" t="s">
         <v>391</v>
       </c>
-      <c r="G9" s="322" t="b">
+      <c r="G9" s="317" t="b">
         <v>1</v>
       </c>
       <c r="H9" s="212">
@@ -7794,7 +7797,7 @@
         <v>258</v>
       </c>
       <c r="X9" s="217" t="s">
-        <v>405</v>
+        <v>403</v>
       </c>
       <c r="Y9" s="219" t="b">
         <v>1</v>
@@ -7815,8 +7818,8 @@
         <v>126</v>
       </c>
       <c r="AE9" s="219">
-        <f ca="1">RANDBETWEEN(5,1440)</f>
-        <v>1311</v>
+        <f t="shared" ca="1" si="0"/>
+        <v>1266</v>
       </c>
       <c r="AF9" s="220" t="s">
         <v>347</v>
@@ -7898,336 +7901,336 @@
       </c>
     </row>
     <row r="10" spans="2:57">
-      <c r="B10" s="296" t="s">
+      <c r="B10" s="291" t="s">
         <v>2</v>
       </c>
-      <c r="C10" s="306" t="s">
+      <c r="C10" s="301" t="s">
         <v>118</v>
       </c>
-      <c r="D10" s="311" t="s">
-        <v>126</v>
-      </c>
-      <c r="E10" s="316" t="s">
+      <c r="D10" s="306" t="s">
+        <v>126</v>
+      </c>
+      <c r="E10" s="311" t="s">
         <v>177</v>
       </c>
-      <c r="F10" s="320" t="s">
+      <c r="F10" s="315" t="s">
         <v>391</v>
       </c>
-      <c r="G10" s="322" t="b">
-        <v>1</v>
-      </c>
-      <c r="H10" s="325">
-        <v>1</v>
-      </c>
-      <c r="I10" s="325" t="b">
-        <v>0</v>
-      </c>
-      <c r="J10" s="325" t="s">
+      <c r="G10" s="317" t="b">
+        <v>1</v>
+      </c>
+      <c r="H10" s="320">
+        <v>1</v>
+      </c>
+      <c r="I10" s="320" t="b">
+        <v>0</v>
+      </c>
+      <c r="J10" s="320" t="s">
         <v>274</v>
       </c>
-      <c r="K10" s="325">
-        <v>1</v>
-      </c>
-      <c r="L10" s="325" t="s">
+      <c r="K10" s="320">
+        <v>1</v>
+      </c>
+      <c r="L10" s="320" t="s">
         <v>275</v>
       </c>
-      <c r="M10" s="325" t="s">
+      <c r="M10" s="320" t="s">
         <v>17</v>
       </c>
-      <c r="N10" s="325">
-        <v>1</v>
-      </c>
-      <c r="O10" s="325" t="s">
+      <c r="N10" s="320">
+        <v>1</v>
+      </c>
+      <c r="O10" s="320" t="s">
         <v>283</v>
       </c>
-      <c r="P10" s="325" t="s">
+      <c r="P10" s="320" t="s">
         <v>17</v>
       </c>
-      <c r="Q10" s="325">
-        <v>1</v>
-      </c>
-      <c r="R10" s="325" t="s">
+      <c r="Q10" s="320">
+        <v>1</v>
+      </c>
+      <c r="R10" s="320" t="s">
         <v>217</v>
       </c>
-      <c r="S10" s="334">
-        <v>0</v>
-      </c>
-      <c r="T10" s="338" t="s">
+      <c r="S10" s="329">
+        <v>0</v>
+      </c>
+      <c r="T10" s="333" t="s">
         <v>103</v>
       </c>
       <c r="U10" s="214" t="s">
         <v>293</v>
       </c>
-      <c r="V10" s="344">
+      <c r="V10" s="339">
         <v>0.7</v>
       </c>
-      <c r="W10" s="349" t="s">
+      <c r="W10" s="344" t="s">
         <v>92</v>
       </c>
-      <c r="X10" s="354" t="s">
+      <c r="X10" s="349" t="s">
         <v>395</v>
       </c>
       <c r="Y10" s="233" t="b">
         <v>1</v>
       </c>
-      <c r="Z10" s="359" t="s">
-        <v>126</v>
-      </c>
-      <c r="AA10" s="359" t="s">
+      <c r="Z10" s="354" t="s">
+        <v>126</v>
+      </c>
+      <c r="AA10" s="354" t="s">
         <v>16</v>
       </c>
-      <c r="AB10" s="359" t="s">
-        <v>126</v>
-      </c>
-      <c r="AC10" s="359" t="s">
-        <v>126</v>
-      </c>
-      <c r="AD10" s="359" t="s">
-        <v>126</v>
-      </c>
-      <c r="AE10" s="359">
-        <f ca="1">RANDBETWEEN(5,1440)</f>
-        <v>1369</v>
+      <c r="AB10" s="354" t="s">
+        <v>126</v>
+      </c>
+      <c r="AC10" s="354" t="s">
+        <v>126</v>
+      </c>
+      <c r="AD10" s="354" t="s">
+        <v>126</v>
+      </c>
+      <c r="AE10" s="354">
+        <f t="shared" ca="1" si="0"/>
+        <v>695</v>
       </c>
       <c r="AF10" s="220" t="s">
         <v>347</v>
       </c>
-      <c r="AG10" s="365" t="s">
-        <v>126</v>
-      </c>
-      <c r="AH10" s="365" t="s">
+      <c r="AG10" s="360" t="s">
+        <v>126</v>
+      </c>
+      <c r="AH10" s="360" t="s">
         <v>126</v>
       </c>
       <c r="AI10" s="220">
         <v>0</v>
       </c>
-      <c r="AJ10" s="365" t="s">
-        <v>126</v>
-      </c>
-      <c r="AK10" s="365" t="s">
-        <v>126</v>
-      </c>
-      <c r="AL10" s="365" t="s">
-        <v>126</v>
-      </c>
-      <c r="AM10" s="365" t="s">
-        <v>126</v>
-      </c>
-      <c r="AN10" s="365" t="s">
-        <v>126</v>
-      </c>
-      <c r="AO10" s="365" t="s">
-        <v>126</v>
-      </c>
-      <c r="AP10" s="365" t="s">
-        <v>126</v>
-      </c>
-      <c r="AQ10" s="365" t="s">
-        <v>126</v>
-      </c>
-      <c r="AR10" s="365" t="s">
-        <v>126</v>
-      </c>
-      <c r="AS10" s="365" t="s">
-        <v>126</v>
-      </c>
-      <c r="AT10" s="365" t="s">
-        <v>126</v>
-      </c>
-      <c r="AU10" s="365" t="s">
-        <v>126</v>
-      </c>
-      <c r="AV10" s="365" t="s">
-        <v>126</v>
-      </c>
-      <c r="AW10" s="365" t="s">
+      <c r="AJ10" s="360" t="s">
+        <v>126</v>
+      </c>
+      <c r="AK10" s="360" t="s">
+        <v>126</v>
+      </c>
+      <c r="AL10" s="360" t="s">
+        <v>126</v>
+      </c>
+      <c r="AM10" s="360" t="s">
+        <v>126</v>
+      </c>
+      <c r="AN10" s="360" t="s">
+        <v>126</v>
+      </c>
+      <c r="AO10" s="360" t="s">
+        <v>126</v>
+      </c>
+      <c r="AP10" s="360" t="s">
+        <v>126</v>
+      </c>
+      <c r="AQ10" s="360" t="s">
+        <v>126</v>
+      </c>
+      <c r="AR10" s="360" t="s">
+        <v>126</v>
+      </c>
+      <c r="AS10" s="360" t="s">
+        <v>126</v>
+      </c>
+      <c r="AT10" s="360" t="s">
+        <v>126</v>
+      </c>
+      <c r="AU10" s="360" t="s">
+        <v>126</v>
+      </c>
+      <c r="AV10" s="360" t="s">
+        <v>126</v>
+      </c>
+      <c r="AW10" s="360" t="s">
         <v>126</v>
       </c>
       <c r="AX10" s="221" t="s">
         <v>396</v>
       </c>
-      <c r="AY10" s="365" t="s">
-        <v>126</v>
-      </c>
-      <c r="AZ10" s="365" t="s">
-        <v>126</v>
-      </c>
-      <c r="BA10" s="365" t="s">
-        <v>126</v>
-      </c>
-      <c r="BB10" s="365" t="s">
-        <v>126</v>
-      </c>
-      <c r="BC10" s="365" t="s">
-        <v>126</v>
-      </c>
-      <c r="BD10" s="365" t="s">
-        <v>126</v>
-      </c>
-      <c r="BE10" s="365" t="s">
+      <c r="AY10" s="360" t="s">
+        <v>126</v>
+      </c>
+      <c r="AZ10" s="360" t="s">
+        <v>126</v>
+      </c>
+      <c r="BA10" s="360" t="s">
+        <v>126</v>
+      </c>
+      <c r="BB10" s="360" t="s">
+        <v>126</v>
+      </c>
+      <c r="BC10" s="360" t="s">
+        <v>126</v>
+      </c>
+      <c r="BD10" s="360" t="s">
+        <v>126</v>
+      </c>
+      <c r="BE10" s="360" t="s">
         <v>126</v>
       </c>
     </row>
     <row r="11" spans="2:57">
-      <c r="B11" s="292" t="s">
+      <c r="B11" s="287" t="s">
         <v>2</v>
       </c>
-      <c r="C11" s="301" t="s">
+      <c r="C11" s="296" t="s">
         <v>122</v>
       </c>
-      <c r="D11" s="309" t="s">
-        <v>126</v>
-      </c>
-      <c r="E11" s="314" t="s">
+      <c r="D11" s="304" t="s">
+        <v>126</v>
+      </c>
+      <c r="E11" s="309" t="s">
         <v>177</v>
       </c>
       <c r="F11" s="225" t="s">
         <v>391</v>
       </c>
-      <c r="G11" s="322" t="b">
-        <v>1</v>
-      </c>
-      <c r="H11" s="322">
-        <v>1</v>
-      </c>
-      <c r="I11" s="322" t="b">
-        <v>0</v>
-      </c>
-      <c r="J11" s="322" t="s">
+      <c r="G11" s="317" t="b">
+        <v>1</v>
+      </c>
+      <c r="H11" s="317">
+        <v>1</v>
+      </c>
+      <c r="I11" s="317" t="b">
+        <v>0</v>
+      </c>
+      <c r="J11" s="317" t="s">
         <v>274</v>
       </c>
-      <c r="K11" s="322">
-        <v>1</v>
-      </c>
-      <c r="L11" s="322" t="s">
+      <c r="K11" s="317">
+        <v>1</v>
+      </c>
+      <c r="L11" s="317" t="s">
         <v>288</v>
       </c>
-      <c r="M11" s="322" t="s">
+      <c r="M11" s="317" t="s">
         <v>12</v>
       </c>
-      <c r="N11" s="322">
+      <c r="N11" s="317">
         <v>50000</v>
       </c>
-      <c r="O11" s="322"/>
-      <c r="P11" s="322"/>
-      <c r="Q11" s="322"/>
-      <c r="R11" s="322"/>
+      <c r="O11" s="317"/>
+      <c r="P11" s="317"/>
+      <c r="Q11" s="317"/>
+      <c r="R11" s="317"/>
       <c r="S11" s="213">
         <v>2</v>
       </c>
-      <c r="T11" s="278" t="s">
+      <c r="T11" s="273" t="s">
         <v>101</v>
       </c>
       <c r="U11" s="214" t="s">
         <v>293</v>
       </c>
-      <c r="V11" s="341">
+      <c r="V11" s="336">
         <v>0.3</v>
       </c>
-      <c r="W11" s="346" t="s">
+      <c r="W11" s="341" t="s">
         <v>96</v>
       </c>
-      <c r="X11" s="351" t="s">
-        <v>399</v>
+      <c r="X11" s="346" t="s">
+        <v>398</v>
       </c>
       <c r="Y11" s="233" t="b">
         <v>1</v>
       </c>
-      <c r="Z11" s="357" t="s">
-        <v>126</v>
-      </c>
-      <c r="AA11" s="357" t="s">
+      <c r="Z11" s="352" t="s">
+        <v>126</v>
+      </c>
+      <c r="AA11" s="352" t="s">
         <v>16</v>
       </c>
-      <c r="AB11" s="357" t="s">
-        <v>126</v>
-      </c>
-      <c r="AC11" s="357" t="s">
-        <v>126</v>
-      </c>
-      <c r="AD11" s="357" t="s">
-        <v>126</v>
-      </c>
-      <c r="AE11" s="357">
-        <f ca="1">RANDBETWEEN(5,1440)</f>
-        <v>243</v>
+      <c r="AB11" s="352" t="s">
+        <v>126</v>
+      </c>
+      <c r="AC11" s="352" t="s">
+        <v>126</v>
+      </c>
+      <c r="AD11" s="352" t="s">
+        <v>126</v>
+      </c>
+      <c r="AE11" s="352">
+        <f t="shared" ca="1" si="0"/>
+        <v>25</v>
       </c>
       <c r="AF11" s="220" t="s">
         <v>347</v>
       </c>
-      <c r="AG11" s="289" t="s">
-        <v>126</v>
-      </c>
-      <c r="AH11" s="289" t="s">
+      <c r="AG11" s="284" t="s">
+        <v>126</v>
+      </c>
+      <c r="AH11" s="284" t="s">
         <v>126</v>
       </c>
       <c r="AI11" s="220">
         <v>0</v>
       </c>
-      <c r="AJ11" s="289" t="s">
-        <v>126</v>
-      </c>
-      <c r="AK11" s="289" t="s">
-        <v>126</v>
-      </c>
-      <c r="AL11" s="289" t="s">
-        <v>126</v>
-      </c>
-      <c r="AM11" s="289" t="s">
-        <v>126</v>
-      </c>
-      <c r="AN11" s="289" t="s">
-        <v>126</v>
-      </c>
-      <c r="AO11" s="289" t="s">
-        <v>126</v>
-      </c>
-      <c r="AP11" s="289" t="s">
-        <v>126</v>
-      </c>
-      <c r="AQ11" s="289" t="s">
-        <v>126</v>
-      </c>
-      <c r="AR11" s="289" t="s">
-        <v>126</v>
-      </c>
-      <c r="AS11" s="289" t="s">
-        <v>126</v>
-      </c>
-      <c r="AT11" s="289" t="s">
-        <v>126</v>
-      </c>
-      <c r="AU11" s="289" t="s">
-        <v>126</v>
-      </c>
-      <c r="AV11" s="289" t="s">
-        <v>126</v>
-      </c>
-      <c r="AW11" s="289" t="s">
+      <c r="AJ11" s="284" t="s">
+        <v>126</v>
+      </c>
+      <c r="AK11" s="284" t="s">
+        <v>126</v>
+      </c>
+      <c r="AL11" s="284" t="s">
+        <v>126</v>
+      </c>
+      <c r="AM11" s="284" t="s">
+        <v>126</v>
+      </c>
+      <c r="AN11" s="284" t="s">
+        <v>126</v>
+      </c>
+      <c r="AO11" s="284" t="s">
+        <v>126</v>
+      </c>
+      <c r="AP11" s="284" t="s">
+        <v>126</v>
+      </c>
+      <c r="AQ11" s="284" t="s">
+        <v>126</v>
+      </c>
+      <c r="AR11" s="284" t="s">
+        <v>126</v>
+      </c>
+      <c r="AS11" s="284" t="s">
+        <v>126</v>
+      </c>
+      <c r="AT11" s="284" t="s">
+        <v>126</v>
+      </c>
+      <c r="AU11" s="284" t="s">
+        <v>126</v>
+      </c>
+      <c r="AV11" s="284" t="s">
+        <v>126</v>
+      </c>
+      <c r="AW11" s="284" t="s">
         <v>126</v>
       </c>
       <c r="AX11" s="221" t="s">
         <v>396</v>
       </c>
-      <c r="AY11" s="289" t="s">
-        <v>126</v>
-      </c>
-      <c r="AZ11" s="289" t="s">
-        <v>126</v>
-      </c>
-      <c r="BA11" s="289" t="s">
-        <v>126</v>
-      </c>
-      <c r="BB11" s="289" t="s">
-        <v>126</v>
-      </c>
-      <c r="BC11" s="289" t="s">
-        <v>126</v>
-      </c>
-      <c r="BD11" s="289" t="s">
-        <v>126</v>
-      </c>
-      <c r="BE11" s="289" t="s">
+      <c r="AY11" s="284" t="s">
+        <v>126</v>
+      </c>
+      <c r="AZ11" s="284" t="s">
+        <v>126</v>
+      </c>
+      <c r="BA11" s="284" t="s">
+        <v>126</v>
+      </c>
+      <c r="BB11" s="284" t="s">
+        <v>126</v>
+      </c>
+      <c r="BC11" s="284" t="s">
+        <v>126</v>
+      </c>
+      <c r="BD11" s="284" t="s">
+        <v>126</v>
+      </c>
+      <c r="BE11" s="284" t="s">
         <v>126</v>
       </c>
     </row>
@@ -8263,7 +8266,7 @@
         <v>1</v>
       </c>
       <c r="L12" s="212" t="s">
-        <v>362</v>
+        <v>405</v>
       </c>
       <c r="M12" s="212" t="s">
         <v>49</v>
@@ -8272,7 +8275,7 @@
         <v>1</v>
       </c>
       <c r="O12" s="212" t="s">
-        <v>397</v>
+        <v>406</v>
       </c>
       <c r="P12" s="212" t="s">
         <v>49</v>
@@ -8281,7 +8284,7 @@
         <v>1</v>
       </c>
       <c r="R12" s="212" t="s">
-        <v>354</v>
+        <v>407</v>
       </c>
       <c r="S12" s="213">
         <v>1</v>
@@ -8299,7 +8302,7 @@
         <v>97</v>
       </c>
       <c r="X12" s="217" t="s">
-        <v>398</v>
+        <v>397</v>
       </c>
       <c r="Y12" s="233" t="b">
         <v>1</v>
@@ -8320,8 +8323,8 @@
         <v>126</v>
       </c>
       <c r="AE12" s="219">
-        <f ca="1">RANDBETWEEN(5,1440)</f>
-        <v>553</v>
+        <f t="shared" ca="1" si="0"/>
+        <v>1091</v>
       </c>
       <c r="AF12" s="220" t="s">
         <v>347</v>
@@ -8460,7 +8463,7 @@
         <v>98</v>
       </c>
       <c r="X13" s="217" t="s">
-        <v>406</v>
+        <v>404</v>
       </c>
       <c r="Y13" s="233" t="b">
         <v>1</v>
@@ -8481,8 +8484,8 @@
         <v>126</v>
       </c>
       <c r="AE13" s="219">
-        <f ca="1">RANDBETWEEN(5,1440)</f>
-        <v>369</v>
+        <f t="shared" ca="1" si="0"/>
+        <v>204</v>
       </c>
       <c r="AF13" s="220" t="s">
         <v>347</v>
@@ -8595,7 +8598,7 @@
         <v>1</v>
       </c>
       <c r="L14" s="212" t="s">
-        <v>357</v>
+        <v>350</v>
       </c>
       <c r="M14" s="212" t="s">
         <v>49</v>
@@ -8604,7 +8607,7 @@
         <v>1</v>
       </c>
       <c r="O14" s="212" t="s">
-        <v>358</v>
+        <v>349</v>
       </c>
       <c r="P14" s="212" t="s">
         <v>49</v>
@@ -8613,7 +8616,7 @@
         <v>1</v>
       </c>
       <c r="R14" s="212" t="s">
-        <v>400</v>
+        <v>351</v>
       </c>
       <c r="S14" s="213">
         <v>3</v>
@@ -8631,7 +8634,7 @@
         <v>99</v>
       </c>
       <c r="X14" s="217" t="s">
-        <v>401</v>
+        <v>399</v>
       </c>
       <c r="Y14" s="218" t="b">
         <v>1</v>
@@ -8652,8 +8655,8 @@
         <v>126</v>
       </c>
       <c r="AE14" s="219">
-        <f ca="1">RANDBETWEEN(5,1440)</f>
-        <v>138</v>
+        <f t="shared" ca="1" si="0"/>
+        <v>731</v>
       </c>
       <c r="AF14" s="220" t="s">
         <v>347</v>
@@ -8786,7 +8789,7 @@
       <c r="R15" s="227" t="s">
         <v>126</v>
       </c>
-      <c r="S15" s="332">
+      <c r="S15" s="327">
         <v>-24</v>
       </c>
       <c r="T15" s="229" t="s">
@@ -8908,7 +8911,7 @@
       <c r="B16" s="239" t="s">
         <v>2</v>
       </c>
-      <c r="C16" s="271" t="s">
+      <c r="C16" s="266" t="s">
         <v>204</v>
       </c>
       <c r="D16" s="239" t="s">
@@ -8942,7 +8945,7 @@
       <c r="P16" s="240"/>
       <c r="Q16" s="240"/>
       <c r="R16" s="240"/>
-      <c r="S16" s="331">
+      <c r="S16" s="326">
         <v>0</v>
       </c>
       <c r="T16" s="241" t="s">
@@ -8951,7 +8954,7 @@
       <c r="U16" s="241" t="s">
         <v>293</v>
       </c>
-      <c r="V16" s="279" t="s">
+      <c r="V16" s="274" t="s">
         <v>126</v>
       </c>
       <c r="W16" s="242" t="s">
@@ -9061,202 +9064,202 @@
       </c>
     </row>
     <row r="17" spans="2:57" ht="17" thickBot="1">
-      <c r="B17" s="291" t="s">
+      <c r="B17" s="286" t="s">
         <v>2</v>
       </c>
-      <c r="C17" s="298" t="s">
+      <c r="C17" s="293" t="s">
         <v>206</v>
       </c>
-      <c r="D17" s="291" t="s">
-        <v>126</v>
-      </c>
-      <c r="E17" s="291" t="s">
+      <c r="D17" s="286" t="s">
+        <v>126</v>
+      </c>
+      <c r="E17" s="286" t="s">
         <v>178</v>
       </c>
-      <c r="F17" s="318" t="s">
+      <c r="F17" s="313" t="s">
         <v>392</v>
       </c>
-      <c r="G17" s="321" t="b">
-        <v>1</v>
-      </c>
-      <c r="H17" s="321">
+      <c r="G17" s="316" t="b">
+        <v>1</v>
+      </c>
+      <c r="H17" s="316">
         <v>-1</v>
       </c>
-      <c r="I17" s="321" t="b">
-        <v>1</v>
-      </c>
-      <c r="J17" s="321" t="s">
+      <c r="I17" s="316" t="b">
+        <v>1</v>
+      </c>
+      <c r="J17" s="316" t="s">
         <v>12</v>
       </c>
-      <c r="K17" s="321">
+      <c r="K17" s="316">
         <v>100000</v>
       </c>
-      <c r="L17" s="327"/>
-      <c r="M17" s="327"/>
-      <c r="N17" s="327"/>
-      <c r="O17" s="327"/>
-      <c r="P17" s="327"/>
-      <c r="Q17" s="327"/>
-      <c r="R17" s="327"/>
-      <c r="S17" s="330">
-        <v>0</v>
-      </c>
-      <c r="T17" s="336" t="s">
+      <c r="L17" s="322"/>
+      <c r="M17" s="322"/>
+      <c r="N17" s="322"/>
+      <c r="O17" s="322"/>
+      <c r="P17" s="322"/>
+      <c r="Q17" s="322"/>
+      <c r="R17" s="322"/>
+      <c r="S17" s="325">
+        <v>0</v>
+      </c>
+      <c r="T17" s="331" t="s">
         <v>101</v>
       </c>
-      <c r="U17" s="336" t="s">
+      <c r="U17" s="331" t="s">
         <v>293</v>
       </c>
-      <c r="V17" s="340" t="s">
-        <v>126</v>
-      </c>
-      <c r="W17" s="345" t="s">
+      <c r="V17" s="335" t="s">
+        <v>126</v>
+      </c>
+      <c r="W17" s="340" t="s">
         <v>247</v>
       </c>
-      <c r="X17" s="350" t="s">
+      <c r="X17" s="345" t="s">
         <v>220</v>
       </c>
-      <c r="Y17" s="355" t="b">
-        <v>0</v>
-      </c>
-      <c r="Z17" s="355">
-        <v>0</v>
-      </c>
-      <c r="AA17" s="355" t="s">
+      <c r="Y17" s="350" t="b">
+        <v>0</v>
+      </c>
+      <c r="Z17" s="350">
+        <v>0</v>
+      </c>
+      <c r="AA17" s="350" t="s">
         <v>16</v>
       </c>
-      <c r="AB17" s="355" t="s">
-        <v>126</v>
-      </c>
-      <c r="AC17" s="355" t="s">
-        <v>126</v>
-      </c>
-      <c r="AD17" s="355" t="s">
-        <v>126</v>
-      </c>
-      <c r="AE17" s="355">
+      <c r="AB17" s="350" t="s">
+        <v>126</v>
+      </c>
+      <c r="AC17" s="350" t="s">
+        <v>126</v>
+      </c>
+      <c r="AD17" s="350" t="s">
+        <v>126</v>
+      </c>
+      <c r="AE17" s="350">
         <v>5</v>
       </c>
       <c r="AF17" s="245" t="s">
         <v>347</v>
       </c>
-      <c r="AG17" s="362" t="s">
-        <v>126</v>
-      </c>
-      <c r="AH17" s="362" t="s">
+      <c r="AG17" s="357" t="s">
+        <v>126</v>
+      </c>
+      <c r="AH17" s="357" t="s">
         <v>126</v>
       </c>
       <c r="AI17" s="245">
         <v>0</v>
       </c>
-      <c r="AJ17" s="362" t="s">
-        <v>126</v>
-      </c>
-      <c r="AK17" s="362" t="s">
-        <v>126</v>
-      </c>
-      <c r="AL17" s="362" t="s">
-        <v>126</v>
-      </c>
-      <c r="AM17" s="362" t="s">
-        <v>126</v>
-      </c>
-      <c r="AN17" s="362" t="s">
-        <v>126</v>
-      </c>
-      <c r="AO17" s="362" t="s">
-        <v>126</v>
-      </c>
-      <c r="AP17" s="362" t="s">
-        <v>126</v>
-      </c>
-      <c r="AQ17" s="362" t="s">
-        <v>126</v>
-      </c>
-      <c r="AR17" s="362" t="s">
-        <v>126</v>
-      </c>
-      <c r="AS17" s="362" t="s">
-        <v>126</v>
-      </c>
-      <c r="AT17" s="362" t="s">
-        <v>126</v>
-      </c>
-      <c r="AU17" s="362" t="s">
-        <v>126</v>
-      </c>
-      <c r="AV17" s="362" t="s">
-        <v>126</v>
-      </c>
-      <c r="AW17" s="362" t="s">
+      <c r="AJ17" s="357" t="s">
+        <v>126</v>
+      </c>
+      <c r="AK17" s="357" t="s">
+        <v>126</v>
+      </c>
+      <c r="AL17" s="357" t="s">
+        <v>126</v>
+      </c>
+      <c r="AM17" s="357" t="s">
+        <v>126</v>
+      </c>
+      <c r="AN17" s="357" t="s">
+        <v>126</v>
+      </c>
+      <c r="AO17" s="357" t="s">
+        <v>126</v>
+      </c>
+      <c r="AP17" s="357" t="s">
+        <v>126</v>
+      </c>
+      <c r="AQ17" s="357" t="s">
+        <v>126</v>
+      </c>
+      <c r="AR17" s="357" t="s">
+        <v>126</v>
+      </c>
+      <c r="AS17" s="357" t="s">
+        <v>126</v>
+      </c>
+      <c r="AT17" s="357" t="s">
+        <v>126</v>
+      </c>
+      <c r="AU17" s="357" t="s">
+        <v>126</v>
+      </c>
+      <c r="AV17" s="357" t="s">
+        <v>126</v>
+      </c>
+      <c r="AW17" s="357" t="s">
         <v>126</v>
       </c>
       <c r="AX17" s="246" t="s">
         <v>396</v>
       </c>
-      <c r="AY17" s="362" t="s">
-        <v>126</v>
-      </c>
-      <c r="AZ17" s="362" t="s">
-        <v>126</v>
-      </c>
-      <c r="BA17" s="362" t="s">
-        <v>126</v>
-      </c>
-      <c r="BB17" s="362" t="s">
-        <v>126</v>
-      </c>
-      <c r="BC17" s="362" t="s">
-        <v>126</v>
-      </c>
-      <c r="BD17" s="362" t="s">
-        <v>126</v>
-      </c>
-      <c r="BE17" s="362" t="s">
+      <c r="AY17" s="357" t="s">
+        <v>126</v>
+      </c>
+      <c r="AZ17" s="357" t="s">
+        <v>126</v>
+      </c>
+      <c r="BA17" s="357" t="s">
+        <v>126</v>
+      </c>
+      <c r="BB17" s="357" t="s">
+        <v>126</v>
+      </c>
+      <c r="BC17" s="357" t="s">
+        <v>126</v>
+      </c>
+      <c r="BD17" s="357" t="s">
+        <v>126</v>
+      </c>
+      <c r="BE17" s="357" t="s">
         <v>126</v>
       </c>
     </row>
     <row r="18" spans="2:57" ht="17" thickTop="1">
-      <c r="B18" s="294" t="s">
+      <c r="B18" s="289" t="s">
         <v>2</v>
       </c>
-      <c r="C18" s="304" t="s">
+      <c r="C18" s="299" t="s">
         <v>213</v>
       </c>
-      <c r="D18" s="294" t="s">
-        <v>126</v>
-      </c>
-      <c r="E18" s="294" t="s">
+      <c r="D18" s="289" t="s">
+        <v>126</v>
+      </c>
+      <c r="E18" s="289" t="s">
         <v>178</v>
       </c>
-      <c r="F18" s="319" t="s">
+      <c r="F18" s="314" t="s">
         <v>392</v>
       </c>
-      <c r="G18" s="324" t="b">
-        <v>1</v>
-      </c>
-      <c r="H18" s="324">
+      <c r="G18" s="319" t="b">
+        <v>1</v>
+      </c>
+      <c r="H18" s="319">
         <v>-1</v>
       </c>
-      <c r="I18" s="324" t="b">
-        <v>1</v>
-      </c>
-      <c r="J18" s="324" t="s">
+      <c r="I18" s="319" t="b">
+        <v>1</v>
+      </c>
+      <c r="J18" s="319" t="s">
         <v>17</v>
       </c>
-      <c r="K18" s="324">
+      <c r="K18" s="319">
         <v>2</v>
       </c>
-      <c r="L18" s="324" t="s">
+      <c r="L18" s="319" t="s">
         <v>283</v>
       </c>
-      <c r="M18" s="324"/>
-      <c r="N18" s="324"/>
-      <c r="O18" s="324"/>
-      <c r="P18" s="324"/>
-      <c r="Q18" s="324"/>
-      <c r="R18" s="324"/>
-      <c r="S18" s="331">
+      <c r="M18" s="319"/>
+      <c r="N18" s="319"/>
+      <c r="O18" s="319"/>
+      <c r="P18" s="319"/>
+      <c r="Q18" s="319"/>
+      <c r="R18" s="319"/>
+      <c r="S18" s="326">
         <v>0</v>
       </c>
       <c r="T18" s="253" t="s">
@@ -9265,112 +9268,112 @@
       <c r="U18" s="253" t="s">
         <v>293</v>
       </c>
-      <c r="V18" s="343" t="s">
-        <v>126</v>
-      </c>
-      <c r="W18" s="348" t="s">
+      <c r="V18" s="338" t="s">
+        <v>126</v>
+      </c>
+      <c r="W18" s="343" t="s">
         <v>254</v>
       </c>
-      <c r="X18" s="353" t="s">
+      <c r="X18" s="348" t="s">
         <v>220</v>
       </c>
-      <c r="Y18" s="356" t="b">
-        <v>0</v>
-      </c>
-      <c r="Z18" s="356">
-        <v>0</v>
-      </c>
-      <c r="AA18" s="356" t="s">
+      <c r="Y18" s="351" t="b">
+        <v>0</v>
+      </c>
+      <c r="Z18" s="351">
+        <v>0</v>
+      </c>
+      <c r="AA18" s="351" t="s">
         <v>16</v>
       </c>
-      <c r="AB18" s="356" t="s">
-        <v>126</v>
-      </c>
-      <c r="AC18" s="356" t="s">
-        <v>126</v>
-      </c>
-      <c r="AD18" s="356" t="s">
-        <v>126</v>
-      </c>
-      <c r="AE18" s="356">
+      <c r="AB18" s="351" t="s">
+        <v>126</v>
+      </c>
+      <c r="AC18" s="351" t="s">
+        <v>126</v>
+      </c>
+      <c r="AD18" s="351" t="s">
+        <v>126</v>
+      </c>
+      <c r="AE18" s="351">
         <v>5</v>
       </c>
       <c r="AF18" s="245" t="s">
         <v>347</v>
       </c>
-      <c r="AG18" s="364" t="s">
-        <v>126</v>
-      </c>
-      <c r="AH18" s="364" t="s">
+      <c r="AG18" s="359" t="s">
+        <v>126</v>
+      </c>
+      <c r="AH18" s="359" t="s">
         <v>126</v>
       </c>
       <c r="AI18" s="245">
         <v>0</v>
       </c>
-      <c r="AJ18" s="364" t="s">
-        <v>126</v>
-      </c>
-      <c r="AK18" s="364" t="s">
-        <v>126</v>
-      </c>
-      <c r="AL18" s="364" t="s">
-        <v>126</v>
-      </c>
-      <c r="AM18" s="364" t="s">
-        <v>126</v>
-      </c>
-      <c r="AN18" s="364" t="s">
-        <v>126</v>
-      </c>
-      <c r="AO18" s="364" t="s">
-        <v>126</v>
-      </c>
-      <c r="AP18" s="364" t="s">
-        <v>126</v>
-      </c>
-      <c r="AQ18" s="364" t="s">
-        <v>126</v>
-      </c>
-      <c r="AR18" s="364" t="s">
-        <v>126</v>
-      </c>
-      <c r="AS18" s="364" t="s">
-        <v>126</v>
-      </c>
-      <c r="AT18" s="364" t="s">
-        <v>126</v>
-      </c>
-      <c r="AU18" s="364" t="s">
-        <v>126</v>
-      </c>
-      <c r="AV18" s="364" t="s">
-        <v>126</v>
-      </c>
-      <c r="AW18" s="364" t="s">
+      <c r="AJ18" s="359" t="s">
+        <v>126</v>
+      </c>
+      <c r="AK18" s="359" t="s">
+        <v>126</v>
+      </c>
+      <c r="AL18" s="359" t="s">
+        <v>126</v>
+      </c>
+      <c r="AM18" s="359" t="s">
+        <v>126</v>
+      </c>
+      <c r="AN18" s="359" t="s">
+        <v>126</v>
+      </c>
+      <c r="AO18" s="359" t="s">
+        <v>126</v>
+      </c>
+      <c r="AP18" s="359" t="s">
+        <v>126</v>
+      </c>
+      <c r="AQ18" s="359" t="s">
+        <v>126</v>
+      </c>
+      <c r="AR18" s="359" t="s">
+        <v>126</v>
+      </c>
+      <c r="AS18" s="359" t="s">
+        <v>126</v>
+      </c>
+      <c r="AT18" s="359" t="s">
+        <v>126</v>
+      </c>
+      <c r="AU18" s="359" t="s">
+        <v>126</v>
+      </c>
+      <c r="AV18" s="359" t="s">
+        <v>126</v>
+      </c>
+      <c r="AW18" s="359" t="s">
         <v>126</v>
       </c>
       <c r="AX18" s="246" t="s">
         <v>396</v>
       </c>
-      <c r="AY18" s="364" t="s">
-        <v>126</v>
-      </c>
-      <c r="AZ18" s="364" t="s">
-        <v>126</v>
-      </c>
-      <c r="BA18" s="364" t="s">
-        <v>126</v>
-      </c>
-      <c r="BB18" s="364" t="s">
-        <v>126</v>
-      </c>
-      <c r="BC18" s="364" t="s">
-        <v>126</v>
-      </c>
-      <c r="BD18" s="364" t="s">
-        <v>126</v>
-      </c>
-      <c r="BE18" s="364" t="s">
+      <c r="AY18" s="359" t="s">
+        <v>126</v>
+      </c>
+      <c r="AZ18" s="359" t="s">
+        <v>126</v>
+      </c>
+      <c r="BA18" s="359" t="s">
+        <v>126</v>
+      </c>
+      <c r="BB18" s="359" t="s">
+        <v>126</v>
+      </c>
+      <c r="BC18" s="359" t="s">
+        <v>126</v>
+      </c>
+      <c r="BD18" s="359" t="s">
+        <v>126</v>
+      </c>
+      <c r="BE18" s="359" t="s">
         <v>126</v>
       </c>
     </row>
@@ -9378,7 +9381,7 @@
       <c r="B19" s="239" t="s">
         <v>2</v>
       </c>
-      <c r="C19" s="271" t="s">
+      <c r="C19" s="266" t="s">
         <v>214</v>
       </c>
       <c r="D19" s="239" t="s">
@@ -9414,7 +9417,7 @@
       <c r="P19" s="240"/>
       <c r="Q19" s="240"/>
       <c r="R19" s="240"/>
-      <c r="S19" s="331">
+      <c r="S19" s="326">
         <v>0</v>
       </c>
       <c r="T19" s="241" t="s">
@@ -9423,7 +9426,7 @@
       <c r="U19" s="241" t="s">
         <v>293</v>
       </c>
-      <c r="V19" s="279" t="s">
+      <c r="V19" s="274" t="s">
         <v>126</v>
       </c>
       <c r="W19" s="242" t="s">
@@ -9536,7 +9539,7 @@
       <c r="B20" s="239" t="s">
         <v>2</v>
       </c>
-      <c r="C20" s="271" t="s">
+      <c r="C20" s="266" t="s">
         <v>215</v>
       </c>
       <c r="D20" s="239" t="s">
@@ -9572,7 +9575,7 @@
       <c r="P20" s="240"/>
       <c r="Q20" s="240"/>
       <c r="R20" s="240"/>
-      <c r="S20" s="331">
+      <c r="S20" s="326">
         <v>0</v>
       </c>
       <c r="T20" s="241">
@@ -9581,7 +9584,7 @@
       <c r="U20" s="241" t="s">
         <v>10</v>
       </c>
-      <c r="V20" s="279" t="s">
+      <c r="V20" s="274" t="s">
         <v>126</v>
       </c>
       <c r="W20" s="242" t="s">
@@ -12356,10 +12359,10 @@
       <c r="B38" s="196" t="s">
         <v>2</v>
       </c>
-      <c r="C38" s="297" t="s">
+      <c r="C38" s="292" t="s">
         <v>116</v>
       </c>
-      <c r="D38" s="312" t="s">
+      <c r="D38" s="307" t="s">
         <v>126</v>
       </c>
       <c r="E38" s="54" t="s">
@@ -12508,13 +12511,13 @@
       <c r="B39" s="67" t="s">
         <v>2</v>
       </c>
-      <c r="C39" s="303" t="s">
+      <c r="C39" s="298" t="s">
         <v>268</v>
       </c>
       <c r="D39" s="67" t="s">
         <v>126</v>
       </c>
-      <c r="E39" s="315" t="s">
+      <c r="E39" s="310" t="s">
         <v>177</v>
       </c>
       <c r="F39" s="188" t="s">
@@ -13266,13 +13269,13 @@
       <c r="B44" s="54" t="s">
         <v>2</v>
       </c>
-      <c r="C44" s="307" t="s">
+      <c r="C44" s="302" t="s">
         <v>266</v>
       </c>
       <c r="D44" s="54" t="s">
         <v>126</v>
       </c>
-      <c r="E44" s="317" t="s">
+      <c r="E44" s="312" t="s">
         <v>177</v>
       </c>
       <c r="F44" s="194" t="s">
@@ -13418,13 +13421,13 @@
       <c r="B45" s="85" t="s">
         <v>2</v>
       </c>
-      <c r="C45" s="299" t="s">
+      <c r="C45" s="294" t="s">
         <v>267</v>
       </c>
       <c r="D45" s="85" t="s">
         <v>126</v>
       </c>
-      <c r="E45" s="313" t="s">
+      <c r="E45" s="308" t="s">
         <v>177</v>
       </c>
       <c r="F45" s="189" t="s">
@@ -14175,16 +14178,16 @@
       </c>
     </row>
     <row r="50" spans="2:57">
-      <c r="B50" s="295" t="s">
+      <c r="B50" s="290" t="s">
         <v>2</v>
       </c>
-      <c r="C50" s="305" t="s">
+      <c r="C50" s="300" t="s">
         <v>343</v>
       </c>
-      <c r="D50" s="310" t="s">
+      <c r="D50" s="305" t="s">
         <v>343</v>
       </c>
-      <c r="E50" s="270" t="s">
+      <c r="E50" s="265" t="s">
         <v>177</v>
       </c>
       <c r="F50" s="194" t="s">
@@ -14193,25 +14196,25 @@
       <c r="G50" s="29" t="b">
         <v>0</v>
       </c>
-      <c r="H50" s="261">
-        <v>1</v>
-      </c>
-      <c r="I50" s="262" t="b">
-        <v>0</v>
-      </c>
-      <c r="J50" s="262"/>
-      <c r="K50" s="262"/>
-      <c r="L50" s="262"/>
-      <c r="M50" s="263"/>
-      <c r="N50" s="263"/>
-      <c r="O50" s="263"/>
-      <c r="P50" s="264"/>
-      <c r="Q50" s="264"/>
-      <c r="R50" s="264"/>
+      <c r="H50" s="256">
+        <v>1</v>
+      </c>
+      <c r="I50" s="257" t="b">
+        <v>0</v>
+      </c>
+      <c r="J50" s="257"/>
+      <c r="K50" s="257"/>
+      <c r="L50" s="257"/>
+      <c r="M50" s="258"/>
+      <c r="N50" s="258"/>
+      <c r="O50" s="258"/>
+      <c r="P50" s="259"/>
+      <c r="Q50" s="259"/>
+      <c r="R50" s="259"/>
       <c r="S50" s="46">
         <v>1</v>
       </c>
-      <c r="T50" s="265" t="s">
+      <c r="T50" s="260" t="s">
         <v>102</v>
       </c>
       <c r="U50" s="47" t="s">
@@ -14220,28 +14223,28 @@
       <c r="V50" s="66" t="s">
         <v>336</v>
       </c>
-      <c r="W50" s="266" t="s">
+      <c r="W50" s="261" t="s">
         <v>340</v>
       </c>
-      <c r="X50" s="267" t="s">
+      <c r="X50" s="262" t="s">
         <v>29</v>
       </c>
-      <c r="Y50" s="282" t="b">
-        <v>1</v>
-      </c>
-      <c r="Z50" s="282">
-        <v>0</v>
-      </c>
-      <c r="AA50" s="282" t="s">
+      <c r="Y50" s="277" t="b">
+        <v>1</v>
+      </c>
+      <c r="Z50" s="277">
+        <v>0</v>
+      </c>
+      <c r="AA50" s="277" t="s">
         <v>16</v>
       </c>
-      <c r="AB50" s="282">
+      <c r="AB50" s="277">
         <v>10</v>
       </c>
-      <c r="AC50" s="284" t="s">
-        <v>126</v>
-      </c>
-      <c r="AD50" s="284" t="s">
+      <c r="AC50" s="279" t="s">
+        <v>126</v>
+      </c>
+      <c r="AD50" s="279" t="s">
         <v>126</v>
       </c>
       <c r="AE50" s="37" t="s">
@@ -14250,10 +14253,10 @@
       <c r="AF50" s="13" t="s">
         <v>347</v>
       </c>
-      <c r="AG50" s="287" t="s">
-        <v>126</v>
-      </c>
-      <c r="AH50" s="287" t="s">
+      <c r="AG50" s="282" t="s">
+        <v>126</v>
+      </c>
+      <c r="AH50" s="282" t="s">
         <v>126</v>
       </c>
       <c r="AI50" s="13">
@@ -14268,61 +14271,61 @@
       <c r="AL50" s="13" t="s">
         <v>126</v>
       </c>
-      <c r="AM50" s="287" t="s">
-        <v>126</v>
-      </c>
-      <c r="AN50" s="287" t="s">
-        <v>126</v>
-      </c>
-      <c r="AO50" s="287" t="s">
-        <v>126</v>
-      </c>
-      <c r="AP50" s="287" t="s">
-        <v>126</v>
-      </c>
-      <c r="AQ50" s="287" t="s">
-        <v>126</v>
-      </c>
-      <c r="AR50" s="287" t="s">
-        <v>126</v>
-      </c>
-      <c r="AS50" s="287" t="s">
-        <v>126</v>
-      </c>
-      <c r="AT50" s="287" t="s">
-        <v>126</v>
-      </c>
-      <c r="AU50" s="287" t="s">
-        <v>126</v>
-      </c>
-      <c r="AV50" s="287" t="s">
-        <v>126</v>
-      </c>
-      <c r="AW50" s="287" t="s">
+      <c r="AM50" s="282" t="s">
+        <v>126</v>
+      </c>
+      <c r="AN50" s="282" t="s">
+        <v>126</v>
+      </c>
+      <c r="AO50" s="282" t="s">
+        <v>126</v>
+      </c>
+      <c r="AP50" s="282" t="s">
+        <v>126</v>
+      </c>
+      <c r="AQ50" s="282" t="s">
+        <v>126</v>
+      </c>
+      <c r="AR50" s="282" t="s">
+        <v>126</v>
+      </c>
+      <c r="AS50" s="282" t="s">
+        <v>126</v>
+      </c>
+      <c r="AT50" s="282" t="s">
+        <v>126</v>
+      </c>
+      <c r="AU50" s="282" t="s">
+        <v>126</v>
+      </c>
+      <c r="AV50" s="282" t="s">
+        <v>126</v>
+      </c>
+      <c r="AW50" s="282" t="s">
         <v>126</v>
       </c>
       <c r="AX50" s="20" t="s">
         <v>321</v>
       </c>
-      <c r="AY50" s="287" t="s">
-        <v>126</v>
-      </c>
-      <c r="AZ50" s="287" t="s">
-        <v>126</v>
-      </c>
-      <c r="BA50" s="287" t="s">
+      <c r="AY50" s="282" t="s">
+        <v>126</v>
+      </c>
+      <c r="AZ50" s="282" t="s">
+        <v>126</v>
+      </c>
+      <c r="BA50" s="282" t="s">
         <v>126</v>
       </c>
       <c r="BB50" s="13" t="s">
         <v>126</v>
       </c>
-      <c r="BC50" s="287" t="s">
-        <v>126</v>
-      </c>
-      <c r="BD50" s="287" t="s">
-        <v>126</v>
-      </c>
-      <c r="BE50" s="287" t="s">
+      <c r="BC50" s="282" t="s">
+        <v>126</v>
+      </c>
+      <c r="BD50" s="282" t="s">
+        <v>126</v>
+      </c>
+      <c r="BE50" s="282" t="s">
         <v>126</v>
       </c>
     </row>
@@ -14330,10 +14333,10 @@
       <c r="B51" s="144" t="s">
         <v>2</v>
       </c>
-      <c r="C51" s="300" t="s">
+      <c r="C51" s="295" t="s">
         <v>344</v>
       </c>
-      <c r="D51" s="308" t="s">
+      <c r="D51" s="303" t="s">
         <v>344</v>
       </c>
       <c r="E51" s="67" t="s">
@@ -14375,7 +14378,7 @@
       <c r="W51" s="73" t="s">
         <v>341</v>
       </c>
-      <c r="X51" s="268" t="s">
+      <c r="X51" s="263" t="s">
         <v>29</v>
       </c>
       <c r="Y51" s="74" t="b">
@@ -14453,7 +14456,7 @@
       <c r="AW51" s="76" t="s">
         <v>126</v>
       </c>
-      <c r="AX51" s="290" t="s">
+      <c r="AX51" s="285" t="s">
         <v>321</v>
       </c>
       <c r="AY51" s="76" t="s">
@@ -14634,7 +14637,7 @@
       <c r="B53" s="27" t="s">
         <v>2</v>
       </c>
-      <c r="C53" s="297" t="s">
+      <c r="C53" s="292" t="s">
         <v>111</v>
       </c>
       <c r="D53" s="24" t="s">
@@ -14786,7 +14789,7 @@
       <c r="B54" s="27" t="s">
         <v>2</v>
       </c>
-      <c r="C54" s="297" t="s">
+      <c r="C54" s="292" t="s">
         <v>112</v>
       </c>
       <c r="D54" s="24" t="s">
@@ -14938,7 +14941,7 @@
       <c r="B55" s="27" t="s">
         <v>2</v>
       </c>
-      <c r="C55" s="297" t="s">
+      <c r="C55" s="292" t="s">
         <v>113</v>
       </c>
       <c r="D55" s="24" t="s">
@@ -15087,73 +15090,73 @@
       </c>
     </row>
     <row r="56" spans="2:57" s="247" customFormat="1" ht="17" thickBot="1">
-      <c r="B56" s="269" t="s">
+      <c r="B56" s="264" t="s">
         <v>2</v>
       </c>
-      <c r="C56" s="272" t="s">
+      <c r="C56" s="267" t="s">
         <v>330</v>
       </c>
-      <c r="D56" s="269" t="s">
-        <v>126</v>
-      </c>
-      <c r="E56" s="269" t="s">
+      <c r="D56" s="264" t="s">
+        <v>126</v>
+      </c>
+      <c r="E56" s="264" t="s">
         <v>322</v>
       </c>
       <c r="F56" s="194" t="s">
         <v>393</v>
       </c>
-      <c r="G56" s="273" t="b">
-        <v>0</v>
-      </c>
-      <c r="H56" s="273">
+      <c r="G56" s="268" t="b">
+        <v>0</v>
+      </c>
+      <c r="H56" s="268">
         <v>1</v>
       </c>
       <c r="I56" s="177" t="s">
         <v>126</v>
       </c>
-      <c r="J56" s="274" t="s">
+      <c r="J56" s="269" t="s">
         <v>322</v>
       </c>
-      <c r="K56" s="274" t="s">
+      <c r="K56" s="269" t="s">
         <v>126</v>
       </c>
       <c r="L56" s="157" t="s">
         <v>126</v>
       </c>
-      <c r="M56" s="275" t="s">
-        <v>126</v>
-      </c>
-      <c r="N56" s="275" t="s">
+      <c r="M56" s="270" t="s">
+        <v>126</v>
+      </c>
+      <c r="N56" s="270" t="s">
         <v>126</v>
       </c>
       <c r="O56" s="158" t="s">
         <v>126</v>
       </c>
-      <c r="P56" s="276" t="s">
-        <v>126</v>
-      </c>
-      <c r="Q56" s="276" t="s">
-        <v>126</v>
-      </c>
-      <c r="R56" s="276" t="s">
-        <v>126</v>
-      </c>
-      <c r="S56" s="335">
+      <c r="P56" s="271" t="s">
+        <v>126</v>
+      </c>
+      <c r="Q56" s="271" t="s">
+        <v>126</v>
+      </c>
+      <c r="R56" s="271" t="s">
+        <v>126</v>
+      </c>
+      <c r="S56" s="330">
         <v>-24</v>
       </c>
-      <c r="T56" s="277" t="s">
+      <c r="T56" s="272" t="s">
         <v>339</v>
       </c>
-      <c r="U56" s="339" t="s">
+      <c r="U56" s="334" t="s">
         <v>293</v>
       </c>
       <c r="V56" s="178" t="s">
         <v>126</v>
       </c>
-      <c r="W56" s="280" t="s">
+      <c r="W56" s="275" t="s">
         <v>323</v>
       </c>
-      <c r="X56" s="281" t="s">
+      <c r="X56" s="276" t="s">
         <v>359</v>
       </c>
       <c r="Y56" s="165" t="b">
@@ -15168,10 +15171,10 @@
       <c r="AB56" s="171" t="s">
         <v>126</v>
       </c>
-      <c r="AC56" s="283" t="s">
-        <v>126</v>
-      </c>
-      <c r="AD56" s="285" t="s">
+      <c r="AC56" s="278" t="s">
+        <v>126</v>
+      </c>
+      <c r="AD56" s="280" t="s">
         <v>126</v>
       </c>
       <c r="AE56" s="167" t="s">
@@ -15180,16 +15183,16 @@
       <c r="AF56" s="168" t="s">
         <v>360</v>
       </c>
-      <c r="AG56" s="286" t="s">
-        <v>126</v>
-      </c>
-      <c r="AH56" s="286" t="s">
+      <c r="AG56" s="281" t="s">
+        <v>126</v>
+      </c>
+      <c r="AH56" s="281" t="s">
         <v>126</v>
       </c>
       <c r="AI56" s="168">
         <v>4</v>
       </c>
-      <c r="AJ56" s="288" t="s">
+      <c r="AJ56" s="283" t="s">
         <v>126</v>
       </c>
       <c r="AK56" s="168" t="s">
@@ -15198,231 +15201,231 @@
       <c r="AL56" s="168" t="s">
         <v>126</v>
       </c>
-      <c r="AM56" s="286" t="s">
-        <v>126</v>
-      </c>
-      <c r="AN56" s="286" t="s">
-        <v>126</v>
-      </c>
-      <c r="AO56" s="286" t="s">
+      <c r="AM56" s="281" t="s">
+        <v>126</v>
+      </c>
+      <c r="AN56" s="281" t="s">
+        <v>126</v>
+      </c>
+      <c r="AO56" s="281" t="s">
         <v>126</v>
       </c>
       <c r="AP56" s="168" t="s">
         <v>126</v>
       </c>
-      <c r="AQ56" s="286" t="s">
-        <v>126</v>
-      </c>
-      <c r="AR56" s="286" t="s">
-        <v>126</v>
-      </c>
-      <c r="AS56" s="286" t="s">
-        <v>126</v>
-      </c>
-      <c r="AT56" s="288" t="s">
-        <v>126</v>
-      </c>
-      <c r="AU56" s="286" t="s">
-        <v>126</v>
-      </c>
-      <c r="AV56" s="286" t="s">
-        <v>126</v>
-      </c>
-      <c r="AW56" s="286" t="s">
+      <c r="AQ56" s="281" t="s">
+        <v>126</v>
+      </c>
+      <c r="AR56" s="281" t="s">
+        <v>126</v>
+      </c>
+      <c r="AS56" s="281" t="s">
+        <v>126</v>
+      </c>
+      <c r="AT56" s="283" t="s">
+        <v>126</v>
+      </c>
+      <c r="AU56" s="281" t="s">
+        <v>126</v>
+      </c>
+      <c r="AV56" s="281" t="s">
+        <v>126</v>
+      </c>
+      <c r="AW56" s="281" t="s">
         <v>126</v>
       </c>
       <c r="AX56" s="168" t="s">
         <v>126</v>
       </c>
-      <c r="AY56" s="286" t="s">
-        <v>126</v>
-      </c>
-      <c r="AZ56" s="286" t="s">
-        <v>126</v>
-      </c>
-      <c r="BA56" s="286" t="s">
+      <c r="AY56" s="281" t="s">
+        <v>126</v>
+      </c>
+      <c r="AZ56" s="281" t="s">
+        <v>126</v>
+      </c>
+      <c r="BA56" s="281" t="s">
         <v>126</v>
       </c>
       <c r="BB56" s="168" t="s">
         <v>126</v>
       </c>
-      <c r="BC56" s="286" t="s">
-        <v>126</v>
-      </c>
-      <c r="BD56" s="286" t="s">
-        <v>126</v>
-      </c>
-      <c r="BE56" s="286" t="s">
+      <c r="BC56" s="281" t="s">
+        <v>126</v>
+      </c>
+      <c r="BD56" s="281" t="s">
+        <v>126</v>
+      </c>
+      <c r="BE56" s="281" t="s">
         <v>126</v>
       </c>
     </row>
     <row r="57" spans="2:57" s="254" customFormat="1" ht="18" thickTop="1" thickBot="1">
-      <c r="B57" s="293" t="s">
+      <c r="B57" s="288" t="s">
         <v>2</v>
       </c>
-      <c r="C57" s="302" t="s">
+      <c r="C57" s="297" t="s">
         <v>331</v>
       </c>
-      <c r="D57" s="293" t="s">
-        <v>126</v>
-      </c>
-      <c r="E57" s="293" t="s">
+      <c r="D57" s="288" t="s">
+        <v>126</v>
+      </c>
+      <c r="E57" s="288" t="s">
         <v>322</v>
       </c>
       <c r="F57" s="189" t="s">
         <v>393</v>
       </c>
-      <c r="G57" s="323" t="b">
-        <v>0</v>
-      </c>
-      <c r="H57" s="323">
-        <v>1</v>
-      </c>
-      <c r="I57" s="326" t="s">
-        <v>126</v>
-      </c>
-      <c r="J57" s="326" t="s">
+      <c r="G57" s="318" t="b">
+        <v>0</v>
+      </c>
+      <c r="H57" s="318">
+        <v>1</v>
+      </c>
+      <c r="I57" s="321" t="s">
+        <v>126</v>
+      </c>
+      <c r="J57" s="321" t="s">
         <v>322</v>
       </c>
-      <c r="K57" s="326" t="s">
-        <v>126</v>
-      </c>
-      <c r="L57" s="326" t="s">
-        <v>126</v>
-      </c>
-      <c r="M57" s="328" t="s">
-        <v>126</v>
-      </c>
-      <c r="N57" s="328" t="s">
-        <v>126</v>
-      </c>
-      <c r="O57" s="328" t="s">
-        <v>126</v>
-      </c>
-      <c r="P57" s="329" t="s">
-        <v>126</v>
-      </c>
-      <c r="Q57" s="329" t="s">
-        <v>126</v>
-      </c>
-      <c r="R57" s="329" t="s">
-        <v>126</v>
-      </c>
-      <c r="S57" s="333">
+      <c r="K57" s="321" t="s">
+        <v>126</v>
+      </c>
+      <c r="L57" s="321" t="s">
+        <v>126</v>
+      </c>
+      <c r="M57" s="323" t="s">
+        <v>126</v>
+      </c>
+      <c r="N57" s="323" t="s">
+        <v>126</v>
+      </c>
+      <c r="O57" s="323" t="s">
+        <v>126</v>
+      </c>
+      <c r="P57" s="324" t="s">
+        <v>126</v>
+      </c>
+      <c r="Q57" s="324" t="s">
+        <v>126</v>
+      </c>
+      <c r="R57" s="324" t="s">
+        <v>126</v>
+      </c>
+      <c r="S57" s="328">
         <v>-24</v>
       </c>
-      <c r="T57" s="337" t="s">
+      <c r="T57" s="332" t="s">
         <v>332</v>
       </c>
-      <c r="U57" s="337" t="s">
+      <c r="U57" s="332" t="s">
         <v>293</v>
       </c>
-      <c r="V57" s="342" t="s">
-        <v>126</v>
-      </c>
-      <c r="W57" s="347" t="s">
+      <c r="V57" s="337" t="s">
+        <v>126</v>
+      </c>
+      <c r="W57" s="342" t="s">
         <v>333</v>
       </c>
-      <c r="X57" s="352" t="s">
+      <c r="X57" s="347" t="s">
         <v>359</v>
       </c>
       <c r="Y57" s="165" t="b">
         <v>0</v>
       </c>
-      <c r="Z57" s="358" t="s">
-        <v>126</v>
-      </c>
-      <c r="AA57" s="358" t="s">
+      <c r="Z57" s="353" t="s">
+        <v>126</v>
+      </c>
+      <c r="AA57" s="353" t="s">
         <v>16</v>
       </c>
-      <c r="AB57" s="358" t="s">
-        <v>126</v>
-      </c>
-      <c r="AC57" s="360" t="s">
-        <v>126</v>
-      </c>
-      <c r="AD57" s="361" t="s">
-        <v>126</v>
-      </c>
-      <c r="AE57" s="361" t="s">
+      <c r="AB57" s="353" t="s">
+        <v>126</v>
+      </c>
+      <c r="AC57" s="355" t="s">
+        <v>126</v>
+      </c>
+      <c r="AD57" s="356" t="s">
+        <v>126</v>
+      </c>
+      <c r="AE57" s="356" t="s">
         <v>126</v>
       </c>
       <c r="AF57" s="168" t="s">
         <v>360</v>
       </c>
-      <c r="AG57" s="363" t="s">
-        <v>126</v>
-      </c>
-      <c r="AH57" s="363" t="s">
+      <c r="AG57" s="358" t="s">
+        <v>126</v>
+      </c>
+      <c r="AH57" s="358" t="s">
         <v>126</v>
       </c>
       <c r="AI57" s="168">
         <v>4</v>
       </c>
-      <c r="AJ57" s="366" t="s">
-        <v>126</v>
-      </c>
-      <c r="AK57" s="363" t="s">
-        <v>126</v>
-      </c>
-      <c r="AL57" s="363" t="s">
-        <v>126</v>
-      </c>
-      <c r="AM57" s="363" t="s">
-        <v>126</v>
-      </c>
-      <c r="AN57" s="363" t="s">
-        <v>126</v>
-      </c>
-      <c r="AO57" s="363" t="s">
-        <v>126</v>
-      </c>
-      <c r="AP57" s="363" t="s">
-        <v>126</v>
-      </c>
-      <c r="AQ57" s="363" t="s">
-        <v>126</v>
-      </c>
-      <c r="AR57" s="363" t="s">
-        <v>126</v>
-      </c>
-      <c r="AS57" s="363" t="s">
-        <v>126</v>
-      </c>
-      <c r="AT57" s="366" t="s">
-        <v>126</v>
-      </c>
-      <c r="AU57" s="363" t="s">
-        <v>126</v>
-      </c>
-      <c r="AV57" s="363" t="s">
-        <v>126</v>
-      </c>
-      <c r="AW57" s="363" t="s">
+      <c r="AJ57" s="361" t="s">
+        <v>126</v>
+      </c>
+      <c r="AK57" s="358" t="s">
+        <v>126</v>
+      </c>
+      <c r="AL57" s="358" t="s">
+        <v>126</v>
+      </c>
+      <c r="AM57" s="358" t="s">
+        <v>126</v>
+      </c>
+      <c r="AN57" s="358" t="s">
+        <v>126</v>
+      </c>
+      <c r="AO57" s="358" t="s">
+        <v>126</v>
+      </c>
+      <c r="AP57" s="358" t="s">
+        <v>126</v>
+      </c>
+      <c r="AQ57" s="358" t="s">
+        <v>126</v>
+      </c>
+      <c r="AR57" s="358" t="s">
+        <v>126</v>
+      </c>
+      <c r="AS57" s="358" t="s">
+        <v>126</v>
+      </c>
+      <c r="AT57" s="361" t="s">
+        <v>126</v>
+      </c>
+      <c r="AU57" s="358" t="s">
+        <v>126</v>
+      </c>
+      <c r="AV57" s="358" t="s">
+        <v>126</v>
+      </c>
+      <c r="AW57" s="358" t="s">
         <v>126</v>
       </c>
       <c r="AX57" s="168" t="s">
         <v>126</v>
       </c>
-      <c r="AY57" s="363" t="s">
-        <v>126</v>
-      </c>
-      <c r="AZ57" s="363" t="s">
-        <v>126</v>
-      </c>
-      <c r="BA57" s="363" t="s">
-        <v>126</v>
-      </c>
-      <c r="BB57" s="363" t="s">
-        <v>126</v>
-      </c>
-      <c r="BC57" s="363" t="s">
-        <v>126</v>
-      </c>
-      <c r="BD57" s="363" t="s">
-        <v>126</v>
-      </c>
-      <c r="BE57" s="363" t="s">
+      <c r="AY57" s="358" t="s">
+        <v>126</v>
+      </c>
+      <c r="AZ57" s="358" t="s">
+        <v>126</v>
+      </c>
+      <c r="BA57" s="358" t="s">
+        <v>126</v>
+      </c>
+      <c r="BB57" s="358" t="s">
+        <v>126</v>
+      </c>
+      <c r="BC57" s="358" t="s">
+        <v>126</v>
+      </c>
+      <c r="BD57" s="358" t="s">
+        <v>126</v>
+      </c>
+      <c r="BE57" s="358" t="s">
         <v>126</v>
       </c>
     </row>
@@ -20499,12 +20502,12 @@
       </c>
     </row>
     <row r="90" spans="2:57" ht="26">
-      <c r="B90" s="258" t="s">
+      <c r="B90" s="364" t="s">
         <v>312</v>
       </c>
-      <c r="C90" s="258"/>
-      <c r="D90" s="258"/>
-      <c r="E90" s="258"/>
+      <c r="C90" s="364"/>
+      <c r="D90" s="364"/>
+      <c r="E90" s="364"/>
     </row>
     <row r="91" spans="2:57" ht="75">
       <c r="J91" s="183"/>
@@ -20723,31 +20726,31 @@
       <c r="T1" s="5"/>
       <c r="U1" s="142"/>
       <c r="V1" s="142"/>
-      <c r="AA1" s="256"/>
-      <c r="AB1" s="256"/>
+      <c r="AA1" s="362"/>
+      <c r="AB1" s="362"/>
       <c r="AC1" s="139"/>
-      <c r="AD1" s="257"/>
-      <c r="AE1" s="257"/>
-      <c r="AF1" s="257"/>
-      <c r="AG1" s="257"/>
-      <c r="AH1" s="257"/>
-      <c r="AI1" s="257"/>
-      <c r="AJ1" s="257"/>
-      <c r="AK1" s="257"/>
-      <c r="AL1" s="257"/>
-      <c r="AM1" s="257"/>
-      <c r="AN1" s="257"/>
-      <c r="AO1" s="257"/>
-      <c r="AP1" s="257"/>
-      <c r="AQ1" s="257"/>
-      <c r="AR1" s="257"/>
-      <c r="AS1" s="257"/>
-      <c r="AT1" s="257"/>
-      <c r="AU1" s="257"/>
-      <c r="AV1" s="257"/>
-      <c r="AW1" s="257"/>
-      <c r="AX1" s="257"/>
-      <c r="AY1" s="257"/>
+      <c r="AD1" s="363"/>
+      <c r="AE1" s="363"/>
+      <c r="AF1" s="363"/>
+      <c r="AG1" s="363"/>
+      <c r="AH1" s="363"/>
+      <c r="AI1" s="363"/>
+      <c r="AJ1" s="363"/>
+      <c r="AK1" s="363"/>
+      <c r="AL1" s="363"/>
+      <c r="AM1" s="363"/>
+      <c r="AN1" s="363"/>
+      <c r="AO1" s="363"/>
+      <c r="AP1" s="363"/>
+      <c r="AQ1" s="363"/>
+      <c r="AR1" s="363"/>
+      <c r="AS1" s="363"/>
+      <c r="AT1" s="363"/>
+      <c r="AU1" s="363"/>
+      <c r="AV1" s="363"/>
+      <c r="AW1" s="363"/>
+      <c r="AX1" s="363"/>
+      <c r="AY1" s="363"/>
     </row>
     <row r="2" spans="2:51" ht="190.5" customHeight="1">
       <c r="B2" s="1" t="s">

</xml_diff>

<commit_message>
Offer Packs: Content - Added a couple of packs with pets.
Former-commit-id: 323fed508a90f329dda19379193b172485c88cd2
</commit_message>
<xml_diff>
--- a/Docs/Content/HungryDragonContent_Offers_SHOP_PLAYTEST.xlsx
+++ b/Docs/Content/HungryDragonContent_Offers_SHOP_PLAYTEST.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/aortin/Documents/UBI/FD/Client_iOS/Docs/Content/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BDC800F1-53AD-754D-96C4-790B6BCF9635}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CAE50733-7CB4-2643-8133-67954D072E1A}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="38400" windowHeight="23540" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="38400" windowHeight="23540" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Packs" sheetId="3" r:id="rId1"/>
@@ -3045,6 +3045,120 @@
         </patternFill>
       </fill>
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left style="thin">
+          <color auto="1"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <scheme val="minor"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="0" tint="-4.9989318521683403E-2"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color auto="1"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <scheme val="minor"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor rgb="FFFFFF00"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <scheme val="minor"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="0" tint="-4.9989318521683403E-2"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
       <border diagonalUp="0" diagonalDown="0">
         <left style="thin">
           <color indexed="64"/>
@@ -3108,120 +3222,6 @@
         <horizontal style="thin">
           <color indexed="64"/>
         </horizontal>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <name val="Calibri"/>
-        <scheme val="minor"/>
-      </font>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="64"/>
-          <bgColor theme="0" tint="-4.9989318521683403E-2"/>
-        </patternFill>
-      </fill>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0" outline="0">
-        <left style="thin">
-          <color auto="1"/>
-        </left>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <name val="Calibri"/>
-        <scheme val="minor"/>
-      </font>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="64"/>
-          <bgColor rgb="FFFFFF00"/>
-        </patternFill>
-      </fill>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0" outline="0">
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <name val="Calibri"/>
-        <scheme val="minor"/>
-      </font>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="64"/>
-          <bgColor theme="0" tint="-4.9989318521683403E-2"/>
-        </patternFill>
-      </fill>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0" outline="0">
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right style="thin">
-          <color auto="1"/>
-        </right>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
       </border>
     </dxf>
     <dxf>
@@ -6189,11 +6189,11 @@
     <tableColumn id="45" xr3:uid="{00000000-0010-0000-0100-00002D000000}" name="[refreshFrequency]" dataDxfId="7"/>
     <tableColumn id="4" xr3:uid="{00000000-0010-0000-0100-000004000000}" name="[rotationalActiveOffers]" dataDxfId="6"/>
     <tableColumn id="5" xr3:uid="{00000000-0010-0000-0100-000005000000}" name="[rotationalHistorySize]" dataDxfId="5"/>
-    <tableColumn id="49" xr3:uid="{00000000-0010-0000-0100-000031000000}" name="[freeHistorySize]" dataDxfId="4"/>
-    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0100-000003000000}" name="[freeCooldownMinutes]" dataDxfId="3"/>
-    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0100-000006000000}" name="[emptyValue]" dataDxfId="2"/>
-    <tableColumn id="7" xr3:uid="{00000000-0010-0000-0100-000007000000}" name="[interstitialsBeforeFirstNoAdsPopup]" dataDxfId="1"/>
-    <tableColumn id="8" xr3:uid="{00000000-0010-0000-0100-000008000000}" name="[interstitialsBetweenNoAdsPopup]" dataDxfId="0"/>
+    <tableColumn id="49" xr3:uid="{00000000-0010-0000-0100-000031000000}" name="[freeHistorySize]" dataDxfId="1"/>
+    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0100-000003000000}" name="[freeCooldownMinutes]" dataDxfId="2"/>
+    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0100-000006000000}" name="[emptyValue]" dataDxfId="0"/>
+    <tableColumn id="7" xr3:uid="{00000000-0010-0000-0100-000007000000}" name="[interstitialsBeforeFirstNoAdsPopup]" dataDxfId="4"/>
+    <tableColumn id="8" xr3:uid="{00000000-0010-0000-0100-000008000000}" name="[interstitialsBetweenNoAdsPopup]" dataDxfId="3"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -6498,8 +6498,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="B1:BE94"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="O17" sqref="O17"/>
+    <sheetView topLeftCell="B73" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="M102" sqref="M102"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16"/>
@@ -7358,7 +7358,7 @@
       </c>
       <c r="AE6" s="216">
         <f t="shared" ref="AE6:AE14" ca="1" si="0">RANDBETWEEN(5,1440)</f>
-        <v>806</v>
+        <v>873</v>
       </c>
       <c r="AF6" s="217" t="s">
         <v>347</v>
@@ -7529,7 +7529,7 @@
       </c>
       <c r="AE7" s="216">
         <f t="shared" ca="1" si="0"/>
-        <v>1439</v>
+        <v>926</v>
       </c>
       <c r="AF7" s="217" t="s">
         <v>347</v>
@@ -7686,7 +7686,7 @@
       </c>
       <c r="AE8" s="216">
         <f t="shared" ca="1" si="0"/>
-        <v>41</v>
+        <v>355</v>
       </c>
       <c r="AF8" s="217" t="s">
         <v>347</v>
@@ -7843,7 +7843,7 @@
       </c>
       <c r="AE9" s="216">
         <f t="shared" ca="1" si="0"/>
-        <v>273</v>
+        <v>421</v>
       </c>
       <c r="AF9" s="217" t="s">
         <v>347</v>
@@ -8014,7 +8014,7 @@
       </c>
       <c r="AE10" s="328">
         <f t="shared" ca="1" si="0"/>
-        <v>1263</v>
+        <v>1212</v>
       </c>
       <c r="AF10" s="217" t="s">
         <v>347</v>
@@ -8177,7 +8177,7 @@
       </c>
       <c r="AE11" s="326">
         <f t="shared" ca="1" si="0"/>
-        <v>699</v>
+        <v>1044</v>
       </c>
       <c r="AF11" s="217" t="s">
         <v>347</v>
@@ -8348,7 +8348,7 @@
       </c>
       <c r="AE12" s="216">
         <f t="shared" ca="1" si="0"/>
-        <v>1404</v>
+        <v>727</v>
       </c>
       <c r="AF12" s="217" t="s">
         <v>347</v>
@@ -8509,7 +8509,7 @@
       </c>
       <c r="AE13" s="216">
         <f t="shared" ca="1" si="0"/>
-        <v>214</v>
+        <v>1407</v>
       </c>
       <c r="AF13" s="217" t="s">
         <v>347</v>
@@ -8680,7 +8680,7 @@
       </c>
       <c r="AE14" s="216">
         <f t="shared" ca="1" si="0"/>
-        <v>1041</v>
+        <v>1156</v>
       </c>
       <c r="AF14" s="217" t="s">
         <v>347</v>
@@ -20722,9 +20722,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:GA57"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="2" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D20" sqref="D20"/>
+      <selection pane="bottomLeft" activeCell="H9" sqref="H9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16"/>

</xml_diff>

<commit_message>
Offer Packs: Content - Reduced rotationals egg amount for faster testing.
Former-commit-id: 26eff327b9050bb6879558bd79957770b6af7162
</commit_message>
<xml_diff>
--- a/Docs/Content/HungryDragonContent_Offers_SHOP_PLAYTEST.xlsx
+++ b/Docs/Content/HungryDragonContent_Offers_SHOP_PLAYTEST.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/aortin/Documents/UBI/FD/Client_iOS/Docs/Content/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CAE50733-7CB4-2643-8133-67954D072E1A}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B9AC9917-173E-7143-825E-1F83B9CEB569}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="38400" windowHeight="23540" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="38400" windowHeight="23540" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Packs" sheetId="3" r:id="rId1"/>
@@ -6498,8 +6498,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="B1:BE94"/>
   <sheetViews>
-    <sheetView topLeftCell="B73" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="M102" sqref="M102"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="K22" sqref="K22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16"/>
@@ -7358,7 +7358,7 @@
       </c>
       <c r="AE6" s="216">
         <f t="shared" ref="AE6:AE14" ca="1" si="0">RANDBETWEEN(5,1440)</f>
-        <v>873</v>
+        <v>642</v>
       </c>
       <c r="AF6" s="217" t="s">
         <v>347</v>
@@ -7529,7 +7529,7 @@
       </c>
       <c r="AE7" s="216">
         <f t="shared" ca="1" si="0"/>
-        <v>926</v>
+        <v>555</v>
       </c>
       <c r="AF7" s="217" t="s">
         <v>347</v>
@@ -7686,7 +7686,7 @@
       </c>
       <c r="AE8" s="216">
         <f t="shared" ca="1" si="0"/>
-        <v>355</v>
+        <v>1063</v>
       </c>
       <c r="AF8" s="217" t="s">
         <v>347</v>
@@ -7843,7 +7843,7 @@
       </c>
       <c r="AE9" s="216">
         <f t="shared" ca="1" si="0"/>
-        <v>421</v>
+        <v>226</v>
       </c>
       <c r="AF9" s="217" t="s">
         <v>347</v>
@@ -8014,7 +8014,7 @@
       </c>
       <c r="AE10" s="328">
         <f t="shared" ca="1" si="0"/>
-        <v>1212</v>
+        <v>237</v>
       </c>
       <c r="AF10" s="217" t="s">
         <v>347</v>
@@ -8177,7 +8177,7 @@
       </c>
       <c r="AE11" s="326">
         <f t="shared" ca="1" si="0"/>
-        <v>1044</v>
+        <v>253</v>
       </c>
       <c r="AF11" s="217" t="s">
         <v>347</v>
@@ -8348,7 +8348,7 @@
       </c>
       <c r="AE12" s="216">
         <f t="shared" ca="1" si="0"/>
-        <v>727</v>
+        <v>917</v>
       </c>
       <c r="AF12" s="217" t="s">
         <v>347</v>
@@ -8509,7 +8509,7 @@
       </c>
       <c r="AE13" s="216">
         <f t="shared" ca="1" si="0"/>
-        <v>1407</v>
+        <v>1311</v>
       </c>
       <c r="AF13" s="217" t="s">
         <v>347</v>
@@ -8680,7 +8680,7 @@
       </c>
       <c r="AE14" s="216">
         <f t="shared" ca="1" si="0"/>
-        <v>1156</v>
+        <v>461</v>
       </c>
       <c r="AF14" s="217" t="s">
         <v>347</v>
@@ -9600,7 +9600,7 @@
         <v>17</v>
       </c>
       <c r="K20" s="237">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="L20" s="237" t="s">
         <v>283</v>
@@ -9758,7 +9758,7 @@
         <v>17</v>
       </c>
       <c r="K21" s="237">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="L21" s="237" t="s">
         <v>217</v>
@@ -9916,7 +9916,7 @@
         <v>17</v>
       </c>
       <c r="K22" s="237">
-        <v>6</v>
+        <v>1</v>
       </c>
       <c r="L22" s="237" t="s">
         <v>216</v>
@@ -20722,7 +20722,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:GA57"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane ySplit="2" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="H9" sqref="H9"/>
     </sheetView>

</xml_diff>